<commit_message>
create a strong energy system
</commit_message>
<xml_diff>
--- a/资料/物品列表20200406.xlsx
+++ b/资料/物品列表20200406.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\86137\Desktop\micro_machinery\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\buildsprogram\javaprogram\micro_machinery\资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E72A41-B84E-4BAF-A7C5-AB74521B37A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B192A2-FA41-4C17-90BA-C89981CF607C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="物品列表" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2586,7 +2586,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2870,32 +2870,32 @@
       <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.08203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.125" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.08203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24" customWidth="1"/>
     <col min="10" max="10" width="13.75" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.4140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.4140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.08203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.4140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.4140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="8" t="s">
         <v>177</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -3338,7 +3338,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -3388,7 +3388,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -3483,7 +3483,7 @@
       </c>
       <c r="R10" s="11"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -3528,7 +3528,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -3601,7 +3601,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -3647,7 +3647,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="9">
         <v>15</v>
       </c>
@@ -3667,7 +3667,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="9">
         <v>16</v>
       </c>
@@ -3687,7 +3687,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="9">
         <v>17</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="9">
         <v>18</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="9">
         <v>20</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -3760,7 +3760,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -3771,7 +3771,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -3793,7 +3793,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="9">
         <v>25</v>
       </c>
@@ -3801,7 +3801,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="9">
         <v>26</v>
       </c>
@@ -3809,7 +3809,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>386</v>
       </c>
@@ -3826,7 +3826,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>537</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>481</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>538</v>
       </c>
@@ -3988,7 +3988,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>568</v>
       </c>
@@ -4038,7 +4038,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>482</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="70" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>483</v>
       </c>
@@ -4138,7 +4138,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
         <v>495</v>
       </c>
@@ -4186,7 +4186,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
         <v>496</v>
       </c>
@@ -4230,7 +4230,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E40" s="9" t="s">
         <v>510</v>
       </c>
@@ -4262,7 +4262,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="G41" s="9" t="s">
         <v>515</v>
       </c>
@@ -4288,7 +4288,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
         <v>498</v>
       </c>
@@ -4305,7 +4305,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
         <v>529</v>
       </c>
@@ -4328,7 +4328,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
         <v>530</v>
       </c>
@@ -4348,7 +4348,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
         <v>531</v>
       </c>
@@ -4365,7 +4365,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
         <v>532</v>
       </c>
@@ -4382,7 +4382,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I47" s="9" t="s">
         <v>561</v>
       </c>
@@ -4390,7 +4390,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I48" s="9" t="s">
         <v>562</v>
       </c>
@@ -4398,7 +4398,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="49" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I49" s="9" t="s">
         <v>563</v>
       </c>
@@ -4406,7 +4406,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="50" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I50" s="9" t="s">
         <v>564</v>
       </c>
@@ -4414,7 +4414,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="51" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I51" s="9" t="s">
         <v>565</v>
       </c>
@@ -4422,7 +4422,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="52" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I52" s="9"/>
     </row>
   </sheetData>
@@ -4437,12 +4437,21 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>574</v>
       </c>
@@ -4453,7 +4462,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -4482,7 +4491,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>604</v>
       </c>
@@ -4511,7 +4520,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -4537,7 +4546,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>577</v>
       </c>
@@ -4563,7 +4572,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>578</v>
       </c>
@@ -4583,7 +4592,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>96</v>
       </c>
@@ -4603,7 +4612,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>82</v>
       </c>
@@ -4629,7 +4638,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>130</v>
       </c>
@@ -4655,7 +4664,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -4681,7 +4690,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -4707,7 +4716,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>584</v>
       </c>
@@ -4736,7 +4745,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>83</v>
       </c>
@@ -4768,7 +4777,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>579</v>
       </c>
@@ -4785,7 +4794,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>414</v>
       </c>
@@ -4802,7 +4811,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>142</v>
       </c>
@@ -4810,7 +4819,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>84</v>
       </c>
@@ -4818,7 +4827,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -4826,7 +4835,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -4834,7 +4843,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>85</v>
       </c>
@@ -4842,7 +4851,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>583</v>
       </c>
@@ -4850,7 +4859,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -4858,7 +4867,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>406</v>
       </c>
@@ -4866,7 +4875,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>137</v>
       </c>
@@ -4874,7 +4883,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>138</v>
       </c>
@@ -4882,7 +4891,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>585</v>
       </c>
@@ -4890,7 +4899,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>413</v>
       </c>
@@ -4898,7 +4907,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>142</v>
       </c>
@@ -4906,7 +4915,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>415</v>
       </c>
@@ -4914,7 +4923,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>144</v>
       </c>
@@ -4937,22 +4946,22 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="19" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>159</v>
       </c>
@@ -5008,7 +5017,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>174</v>
       </c>
@@ -5076,7 +5085,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -5140,7 +5149,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -5192,7 +5201,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -5232,7 +5241,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -5282,7 +5291,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -5334,7 +5343,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -5380,7 +5389,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -5420,7 +5429,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -5450,7 +5459,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -5490,7 +5499,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>62</v>
       </c>
@@ -5531,7 +5540,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>63</v>
       </c>
@@ -5557,7 +5566,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -5584,7 +5593,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -5618,7 +5627,7 @@
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -5654,7 +5663,7 @@
       <c r="U17" s="18"/>
       <c r="V17" s="18"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -5685,7 +5694,7 @@
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>84</v>
       </c>
@@ -5721,7 +5730,7 @@
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -5755,7 +5764,7 @@
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -5783,7 +5792,7 @@
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -5817,7 +5826,7 @@
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -5849,7 +5858,7 @@
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>60</v>
       </c>
@@ -5881,7 +5890,7 @@
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -5911,7 +5920,7 @@
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -5939,7 +5948,7 @@
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>76</v>
       </c>
@@ -5967,7 +5976,7 @@
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>78</v>
       </c>
@@ -5995,7 +6004,7 @@
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -6027,7 +6036,7 @@
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -6055,7 +6064,7 @@
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -6078,7 +6087,7 @@
       <c r="U31" s="2"/>
       <c r="V31" s="2"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>175</v>
       </c>
@@ -6104,7 +6113,7 @@
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -6137,7 +6146,7 @@
       <c r="AB33" s="15"/>
       <c r="AC33" s="15"/>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -6175,7 +6184,7 @@
       <c r="AB34" s="15"/>
       <c r="AC34" s="15"/>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>157</v>
       </c>
@@ -6211,7 +6220,7 @@
       <c r="AB35" s="15"/>
       <c r="AC35" s="15"/>
     </row>
-    <row r="36" spans="1:29" ht="47" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" ht="47.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>66</v>
       </c>
@@ -6247,7 +6256,7 @@
       <c r="AB36" s="15"/>
       <c r="AC36" s="15"/>
     </row>
-    <row r="37" spans="1:29" ht="29.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -6282,7 +6291,7 @@
       <c r="AB37" s="15"/>
       <c r="AC37" s="15"/>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>88</v>
       </c>
@@ -6320,7 +6329,7 @@
       <c r="AB38" s="15"/>
       <c r="AC38" s="15"/>
     </row>
-    <row r="39" spans="1:29" ht="39.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:29" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>92</v>
       </c>
@@ -6359,7 +6368,7 @@
       <c r="AB39" s="15"/>
       <c r="AC39" s="15"/>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
         <v>49</v>
       </c>
@@ -6398,7 +6407,7 @@
       <c r="AB40" s="15"/>
       <c r="AC40" s="15"/>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
         <v>99</v>
       </c>
@@ -6424,7 +6433,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
         <v>102</v>
       </c>
@@ -6455,7 +6464,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
         <v>105</v>
       </c>
@@ -6483,7 +6492,7 @@
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -6505,7 +6514,7 @@
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>107</v>
       </c>
@@ -6532,7 +6541,7 @@
       <c r="T45" s="2"/>
       <c r="U45" s="2"/>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B46" s="13" t="s">
         <v>111</v>
       </c>
@@ -6560,7 +6569,7 @@
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B47" s="13" t="s">
         <v>113</v>
       </c>
@@ -6588,7 +6597,7 @@
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
         <v>117</v>
       </c>
@@ -6616,7 +6625,7 @@
       <c r="T48" s="2"/>
       <c r="U48" s="2"/>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B49" s="2" t="s">
         <v>118</v>
       </c>
@@ -6644,7 +6653,7 @@
       <c r="T49" s="2"/>
       <c r="U49" s="2"/>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B50" s="2" t="s">
         <v>128</v>
       </c>
@@ -6672,7 +6681,7 @@
       <c r="T50" s="2"/>
       <c r="U50" s="2"/>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -6694,7 +6703,7 @@
       <c r="T51" s="2"/>
       <c r="U51" s="2"/>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>145</v>
       </c>
@@ -6729,7 +6738,7 @@
       <c r="T52" s="2"/>
       <c r="U52" s="2"/>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>147</v>
       </c>
@@ -6764,7 +6773,7 @@
       <c r="T53" s="2"/>
       <c r="U53" s="2"/>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>148</v>
       </c>
@@ -6798,7 +6807,7 @@
       <c r="T54" s="2"/>
       <c r="U54" s="2"/>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>149</v>
       </c>
@@ -6832,7 +6841,7 @@
       <c r="T55" s="2"/>
       <c r="U55" s="2"/>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>150</v>
       </c>
@@ -6866,7 +6875,7 @@
       <c r="T56" s="2"/>
       <c r="U56" s="2"/>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>151</v>
       </c>
@@ -6900,7 +6909,7 @@
       <c r="T57" s="2"/>
       <c r="U57" s="2"/>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -6911,7 +6920,7 @@
       <c r="T58" s="2"/>
       <c r="U58" s="2"/>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>119</v>
       </c>
@@ -6938,7 +6947,7 @@
       <c r="T59" s="2"/>
       <c r="U59" s="2"/>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B60" s="4" t="s">
         <v>122</v>
       </c>
@@ -6964,7 +6973,7 @@
       <c r="T60" s="2"/>
       <c r="U60" s="2"/>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B61" s="4" t="s">
         <v>124</v>
       </c>
@@ -6990,7 +6999,7 @@
       <c r="T61" s="2"/>
       <c r="U61" s="2"/>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -7012,7 +7021,7 @@
       <c r="T62" s="2"/>
       <c r="U62" s="2"/>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>129</v>
       </c>
@@ -7041,7 +7050,7 @@
       <c r="T63" s="2"/>
       <c r="U63" s="2"/>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B64" s="2" t="s">
         <v>132</v>
       </c>
@@ -7068,7 +7077,7 @@
       <c r="T64" s="2"/>
       <c r="U64" s="2"/>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B65" s="2" t="s">
         <v>47</v>
       </c>
@@ -7096,7 +7105,7 @@
       <c r="T65" s="2"/>
       <c r="U65" s="2"/>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -7120,7 +7129,7 @@
       <c r="T66" s="2"/>
       <c r="U66" s="2"/>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>134</v>
       </c>
@@ -7149,7 +7158,7 @@
       <c r="T67" s="2"/>
       <c r="U67" s="2"/>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B68" s="2" t="s">
         <v>137</v>
       </c>
@@ -7179,7 +7188,7 @@
       <c r="T68" s="2"/>
       <c r="U68" s="2"/>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B69" s="2" t="s">
         <v>76</v>
       </c>
@@ -7205,7 +7214,7 @@
       <c r="T69" s="2"/>
       <c r="U69" s="2"/>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B70" s="2" t="s">
         <v>83</v>
       </c>
@@ -7231,7 +7240,7 @@
       <c r="T70" s="2"/>
       <c r="U70" s="2"/>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B71" s="12" t="s">
         <v>139</v>
       </c>
@@ -7259,7 +7268,7 @@
       <c r="T71" s="2"/>
       <c r="U71" s="2"/>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B72" s="2" t="s">
         <v>141</v>
       </c>
@@ -7285,7 +7294,7 @@
       <c r="T72" s="2"/>
       <c r="U72" s="2"/>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B73" s="2" t="s">
         <v>143</v>
       </c>
@@ -7313,7 +7322,7 @@
       <c r="T73" s="2"/>
       <c r="U73" s="2"/>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
@@ -7335,7 +7344,7 @@
       <c r="T74" s="2"/>
       <c r="U74" s="2"/>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
@@ -7357,7 +7366,7 @@
       <c r="T75" s="2"/>
       <c r="U75" s="2"/>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
@@ -7379,7 +7388,7 @@
       <c r="T76" s="2"/>
       <c r="U76" s="2"/>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
@@ -7401,7 +7410,7 @@
       <c r="T77" s="2"/>
       <c r="U77" s="2"/>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
@@ -7423,7 +7432,7 @@
       <c r="T78" s="2"/>
       <c r="U78" s="2"/>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
@@ -7445,7 +7454,7 @@
       <c r="T79" s="2"/>
       <c r="U79" s="2"/>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
@@ -7467,7 +7476,7 @@
       <c r="T80" s="2"/>
       <c r="U80" s="2"/>
     </row>
-    <row r="81" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
@@ -7489,7 +7498,7 @@
       <c r="T81" s="2"/>
       <c r="U81" s="2"/>
     </row>
-    <row r="82" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
@@ -7511,7 +7520,7 @@
       <c r="T82" s="2"/>
       <c r="U82" s="2"/>
     </row>
-    <row r="83" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
@@ -7533,7 +7542,7 @@
       <c r="T83" s="2"/>
       <c r="U83" s="2"/>
     </row>
-    <row r="84" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
@@ -7555,7 +7564,7 @@
       <c r="T84" s="2"/>
       <c r="U84" s="2"/>
     </row>
-    <row r="85" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
@@ -7577,7 +7586,7 @@
       <c r="T85" s="2"/>
       <c r="U85" s="2"/>
     </row>
-    <row r="86" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
@@ -7599,7 +7608,7 @@
       <c r="T86" s="2"/>
       <c r="U86" s="2"/>
     </row>
-    <row r="87" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
@@ -7621,7 +7630,7 @@
       <c r="T87" s="2"/>
       <c r="U87" s="2"/>
     </row>
-    <row r="88" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
@@ -7643,7 +7652,7 @@
       <c r="T88" s="2"/>
       <c r="U88" s="2"/>
     </row>
-    <row r="89" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
@@ -7665,7 +7674,7 @@
       <c r="T89" s="2"/>
       <c r="U89" s="2"/>
     </row>
-    <row r="90" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
@@ -7687,7 +7696,7 @@
       <c r="T90" s="2"/>
       <c r="U90" s="2"/>
     </row>
-    <row r="91" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
@@ -7709,7 +7718,7 @@
       <c r="T91" s="2"/>
       <c r="U91" s="2"/>
     </row>
-    <row r="92" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
@@ -7731,7 +7740,7 @@
       <c r="T92" s="2"/>
       <c r="U92" s="2"/>
     </row>
-    <row r="93" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
@@ -7753,7 +7762,7 @@
       <c r="T93" s="2"/>
       <c r="U93" s="2"/>
     </row>
-    <row r="94" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
@@ -7775,7 +7784,7 @@
       <c r="T94" s="2"/>
       <c r="U94" s="2"/>
     </row>
-    <row r="95" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
@@ -7797,7 +7806,7 @@
       <c r="T95" s="2"/>
       <c r="U95" s="2"/>
     </row>
-    <row r="96" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
@@ -7819,7 +7828,7 @@
       <c r="T96" s="2"/>
       <c r="U96" s="2"/>
     </row>
-    <row r="97" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
@@ -7841,7 +7850,7 @@
       <c r="T97" s="2"/>
       <c r="U97" s="2"/>
     </row>
-    <row r="98" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
@@ -7863,7 +7872,7 @@
       <c r="T98" s="2"/>
       <c r="U98" s="2"/>
     </row>
-    <row r="99" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
@@ -7885,7 +7894,7 @@
       <c r="T99" s="2"/>
       <c r="U99" s="2"/>
     </row>
-    <row r="100" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
@@ -7907,7 +7916,7 @@
       <c r="T100" s="2"/>
       <c r="U100" s="2"/>
     </row>
-    <row r="101" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
@@ -7929,7 +7938,7 @@
       <c r="T101" s="2"/>
       <c r="U101" s="2"/>
     </row>
-    <row r="102" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
@@ -7951,7 +7960,7 @@
       <c r="T102" s="2"/>
       <c r="U102" s="2"/>
     </row>
-    <row r="103" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
@@ -7973,7 +7982,7 @@
       <c r="T103" s="2"/>
       <c r="U103" s="2"/>
     </row>
-    <row r="104" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
@@ -7995,7 +8004,7 @@
       <c r="T104" s="2"/>
       <c r="U104" s="2"/>
     </row>
-    <row r="105" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
@@ -8017,7 +8026,7 @@
       <c r="T105" s="2"/>
       <c r="U105" s="2"/>
     </row>
-    <row r="106" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
@@ -8039,7 +8048,7 @@
       <c r="T106" s="2"/>
       <c r="U106" s="2"/>
     </row>
-    <row r="107" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
@@ -8061,7 +8070,7 @@
       <c r="T107" s="2"/>
       <c r="U107" s="2"/>
     </row>
-    <row r="108" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
@@ -8083,7 +8092,7 @@
       <c r="T108" s="2"/>
       <c r="U108" s="2"/>
     </row>
-    <row r="109" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
@@ -8105,7 +8114,7 @@
       <c r="T109" s="2"/>
       <c r="U109" s="2"/>
     </row>
-    <row r="110" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
@@ -8127,7 +8136,7 @@
       <c r="T110" s="2"/>
       <c r="U110" s="2"/>
     </row>
-    <row r="111" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
@@ -8149,7 +8158,7 @@
       <c r="T111" s="2"/>
       <c r="U111" s="2"/>
     </row>
-    <row r="112" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
@@ -8171,7 +8180,7 @@
       <c r="T112" s="2"/>
       <c r="U112" s="2"/>
     </row>
-    <row r="113" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
@@ -8193,7 +8202,7 @@
       <c r="T113" s="2"/>
       <c r="U113" s="2"/>
     </row>
-    <row r="114" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
@@ -8215,7 +8224,7 @@
       <c r="T114" s="2"/>
       <c r="U114" s="2"/>
     </row>
-    <row r="115" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
@@ -8237,7 +8246,7 @@
       <c r="T115" s="2"/>
       <c r="U115" s="2"/>
     </row>
-    <row r="116" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
@@ -8259,7 +8268,7 @@
       <c r="T116" s="2"/>
       <c r="U116" s="2"/>
     </row>
-    <row r="117" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
       <c r="D117" s="2"/>
@@ -8281,7 +8290,7 @@
       <c r="T117" s="2"/>
       <c r="U117" s="2"/>
     </row>
-    <row r="118" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
       <c r="D118" s="2"/>
@@ -8303,7 +8312,7 @@
       <c r="T118" s="2"/>
       <c r="U118" s="2"/>
     </row>
-    <row r="119" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
@@ -8325,7 +8334,7 @@
       <c r="T119" s="2"/>
       <c r="U119" s="2"/>
     </row>
-    <row r="120" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
       <c r="D120" s="2"/>
@@ -8347,7 +8356,7 @@
       <c r="T120" s="2"/>
       <c r="U120" s="2"/>
     </row>
-    <row r="121" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
@@ -8369,7 +8378,7 @@
       <c r="T121" s="2"/>
       <c r="U121" s="2"/>
     </row>
-    <row r="122" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
       <c r="D122" s="2"/>
@@ -8391,7 +8400,7 @@
       <c r="T122" s="2"/>
       <c r="U122" s="2"/>
     </row>
-    <row r="123" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
@@ -8413,7 +8422,7 @@
       <c r="T123" s="2"/>
       <c r="U123" s="2"/>
     </row>
-    <row r="124" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
       <c r="D124" s="2"/>
@@ -8435,7 +8444,7 @@
       <c r="T124" s="2"/>
       <c r="U124" s="2"/>
     </row>
-    <row r="125" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
       <c r="D125" s="2"/>
@@ -8457,7 +8466,7 @@
       <c r="T125" s="2"/>
       <c r="U125" s="2"/>
     </row>
-    <row r="126" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
       <c r="D126" s="2"/>
@@ -8479,7 +8488,7 @@
       <c r="T126" s="2"/>
       <c r="U126" s="2"/>
     </row>
-    <row r="127" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
       <c r="D127" s="2"/>
@@ -8501,7 +8510,7 @@
       <c r="T127" s="2"/>
       <c r="U127" s="2"/>
     </row>
-    <row r="128" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
       <c r="D128" s="2"/>
@@ -8523,7 +8532,7 @@
       <c r="T128" s="2"/>
       <c r="U128" s="2"/>
     </row>
-    <row r="129" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
       <c r="D129" s="2"/>
@@ -8545,7 +8554,7 @@
       <c r="T129" s="2"/>
       <c r="U129" s="2"/>
     </row>
-    <row r="130" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
       <c r="D130" s="2"/>
@@ -8567,7 +8576,7 @@
       <c r="T130" s="2"/>
       <c r="U130" s="2"/>
     </row>
-    <row r="131" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
       <c r="D131" s="2"/>
@@ -8589,7 +8598,7 @@
       <c r="T131" s="2"/>
       <c r="U131" s="2"/>
     </row>
-    <row r="132" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
       <c r="D132" s="2"/>
@@ -8611,7 +8620,7 @@
       <c r="T132" s="2"/>
       <c r="U132" s="2"/>
     </row>
-    <row r="133" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
       <c r="D133" s="2"/>
@@ -8633,7 +8642,7 @@
       <c r="T133" s="2"/>
       <c r="U133" s="2"/>
     </row>
-    <row r="134" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
@@ -8655,7 +8664,7 @@
       <c r="T134" s="2"/>
       <c r="U134" s="2"/>
     </row>
-    <row r="135" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
       <c r="D135" s="2"/>
@@ -8677,7 +8686,7 @@
       <c r="T135" s="2"/>
       <c r="U135" s="2"/>
     </row>
-    <row r="136" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
       <c r="D136" s="2"/>
@@ -8699,7 +8708,7 @@
       <c r="T136" s="2"/>
       <c r="U136" s="2"/>
     </row>
-    <row r="137" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
       <c r="D137" s="2"/>
@@ -8721,7 +8730,7 @@
       <c r="T137" s="2"/>
       <c r="U137" s="2"/>
     </row>
-    <row r="138" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
       <c r="D138" s="2"/>
@@ -8743,7 +8752,7 @@
       <c r="T138" s="2"/>
       <c r="U138" s="2"/>
     </row>
-    <row r="139" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
       <c r="D139" s="2"/>
@@ -8765,7 +8774,7 @@
       <c r="T139" s="2"/>
       <c r="U139" s="2"/>
     </row>
-    <row r="140" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
       <c r="D140" s="2"/>
@@ -8787,7 +8796,7 @@
       <c r="T140" s="2"/>
       <c r="U140" s="2"/>
     </row>
-    <row r="141" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
       <c r="D141" s="2"/>
@@ -8809,7 +8818,7 @@
       <c r="T141" s="2"/>
       <c r="U141" s="2"/>
     </row>
-    <row r="142" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
       <c r="D142" s="2"/>
@@ -8831,7 +8840,7 @@
       <c r="T142" s="2"/>
       <c r="U142" s="2"/>
     </row>
-    <row r="143" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
       <c r="D143" s="2"/>
@@ -8853,7 +8862,7 @@
       <c r="T143" s="2"/>
       <c r="U143" s="2"/>
     </row>
-    <row r="144" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
       <c r="D144" s="2"/>
@@ -8875,7 +8884,7 @@
       <c r="T144" s="2"/>
       <c r="U144" s="2"/>
     </row>
-    <row r="145" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
       <c r="D145" s="2"/>
@@ -8897,7 +8906,7 @@
       <c r="T145" s="2"/>
       <c r="U145" s="2"/>
     </row>
-    <row r="146" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
       <c r="D146" s="2"/>
@@ -8919,7 +8928,7 @@
       <c r="T146" s="2"/>
       <c r="U146" s="2"/>
     </row>
-    <row r="147" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
       <c r="D147" s="2"/>
@@ -8941,7 +8950,7 @@
       <c r="T147" s="2"/>
       <c r="U147" s="2"/>
     </row>
-    <row r="148" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
       <c r="D148" s="2"/>
@@ -8963,7 +8972,7 @@
       <c r="T148" s="2"/>
       <c r="U148" s="2"/>
     </row>
-    <row r="149" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
       <c r="D149" s="2"/>
@@ -8985,7 +8994,7 @@
       <c r="T149" s="2"/>
       <c r="U149" s="2"/>
     </row>
-    <row r="150" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
       <c r="D150" s="2"/>
@@ -9007,7 +9016,7 @@
       <c r="T150" s="2"/>
       <c r="U150" s="2"/>
     </row>
-    <row r="151" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
       <c r="D151" s="2"/>
@@ -9029,7 +9038,7 @@
       <c r="T151" s="2"/>
       <c r="U151" s="2"/>
     </row>
-    <row r="152" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
       <c r="D152" s="2"/>
@@ -9051,7 +9060,7 @@
       <c r="T152" s="2"/>
       <c r="U152" s="2"/>
     </row>
-    <row r="153" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
       <c r="D153" s="2"/>
@@ -9073,7 +9082,7 @@
       <c r="T153" s="2"/>
       <c r="U153" s="2"/>
     </row>
-    <row r="154" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
       <c r="D154" s="2"/>
@@ -9095,7 +9104,7 @@
       <c r="T154" s="2"/>
       <c r="U154" s="2"/>
     </row>
-    <row r="155" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
       <c r="D155" s="2"/>
@@ -9117,7 +9126,7 @@
       <c r="T155" s="2"/>
       <c r="U155" s="2"/>
     </row>
-    <row r="156" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
       <c r="D156" s="2"/>
@@ -9139,7 +9148,7 @@
       <c r="T156" s="2"/>
       <c r="U156" s="2"/>
     </row>
-    <row r="157" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
       <c r="D157" s="2"/>
@@ -9161,7 +9170,7 @@
       <c r="T157" s="2"/>
       <c r="U157" s="2"/>
     </row>
-    <row r="158" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
       <c r="D158" s="2"/>
@@ -9183,7 +9192,7 @@
       <c r="T158" s="2"/>
       <c r="U158" s="2"/>
     </row>
-    <row r="159" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
       <c r="D159" s="2"/>
@@ -9205,7 +9214,7 @@
       <c r="T159" s="2"/>
       <c r="U159" s="2"/>
     </row>
-    <row r="160" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
       <c r="D160" s="2"/>
@@ -9227,7 +9236,7 @@
       <c r="T160" s="2"/>
       <c r="U160" s="2"/>
     </row>
-    <row r="161" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
       <c r="D161" s="2"/>
@@ -9249,7 +9258,7 @@
       <c r="T161" s="2"/>
       <c r="U161" s="2"/>
     </row>
-    <row r="162" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
       <c r="D162" s="2"/>
@@ -9271,7 +9280,7 @@
       <c r="T162" s="2"/>
       <c r="U162" s="2"/>
     </row>
-    <row r="163" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
       <c r="D163" s="2"/>
@@ -9293,7 +9302,7 @@
       <c r="T163" s="2"/>
       <c r="U163" s="2"/>
     </row>
-    <row r="164" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
       <c r="D164" s="2"/>
@@ -9315,7 +9324,7 @@
       <c r="T164" s="2"/>
       <c r="U164" s="2"/>
     </row>
-    <row r="165" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
       <c r="D165" s="2"/>
@@ -9337,7 +9346,7 @@
       <c r="T165" s="2"/>
       <c r="U165" s="2"/>
     </row>
-    <row r="166" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
       <c r="D166" s="2"/>
@@ -9359,7 +9368,7 @@
       <c r="T166" s="2"/>
       <c r="U166" s="2"/>
     </row>
-    <row r="167" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
       <c r="D167" s="2"/>
@@ -9381,7 +9390,7 @@
       <c r="T167" s="2"/>
       <c r="U167" s="2"/>
     </row>
-    <row r="168" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
       <c r="D168" s="2"/>
@@ -9403,7 +9412,7 @@
       <c r="T168" s="2"/>
       <c r="U168" s="2"/>
     </row>
-    <row r="169" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
       <c r="D169" s="2"/>
@@ -9425,7 +9434,7 @@
       <c r="T169" s="2"/>
       <c r="U169" s="2"/>
     </row>
-    <row r="170" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
       <c r="D170" s="2"/>
@@ -9447,7 +9456,7 @@
       <c r="T170" s="2"/>
       <c r="U170" s="2"/>
     </row>
-    <row r="171" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
       <c r="D171" s="2"/>
@@ -9469,7 +9478,7 @@
       <c r="T171" s="2"/>
       <c r="U171" s="2"/>
     </row>
-    <row r="172" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
       <c r="D172" s="2"/>
@@ -9491,7 +9500,7 @@
       <c r="T172" s="2"/>
       <c r="U172" s="2"/>
     </row>
-    <row r="173" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
       <c r="D173" s="2"/>
@@ -9513,7 +9522,7 @@
       <c r="T173" s="2"/>
       <c r="U173" s="2"/>
     </row>
-    <row r="174" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
       <c r="D174" s="2"/>
@@ -9535,7 +9544,7 @@
       <c r="T174" s="2"/>
       <c r="U174" s="2"/>
     </row>
-    <row r="175" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
       <c r="D175" s="2"/>
@@ -9557,7 +9566,7 @@
       <c r="T175" s="2"/>
       <c r="U175" s="2"/>
     </row>
-    <row r="176" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:21" x14ac:dyDescent="0.2">
       <c r="E176" s="2"/>
       <c r="F176" s="2"/>
       <c r="G176" s="2"/>
@@ -9576,7 +9585,7 @@
       <c r="T176" s="2"/>
       <c r="U176" s="2"/>
     </row>
-    <row r="177" spans="14:21" x14ac:dyDescent="0.3">
+    <row r="177" spans="14:21" x14ac:dyDescent="0.2">
       <c r="N177" s="2"/>
       <c r="O177" s="2"/>
       <c r="P177" s="2"/>
@@ -9615,179 +9624,179 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>463</v>
       </c>

</xml_diff>